<commit_message>
Role Based Login Implemented.
</commit_message>
<xml_diff>
--- a/src/addon365.Web.API/Resources/EmployeeTemplate.xlsx
+++ b/src/addon365.Web.API/Resources/EmployeeTemplate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Me\Addon\BikeShowRoom\b1ke-sh0wr00m\src\addon365.Web.API\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D5B46485-CE40-4D41-89F4-13E03A981F73}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1B243CF-42D7-4736-B79D-C4B0FF101B54}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8105" xr2:uid="{4AD98230-DE9E-43EB-897A-5902C318DD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>UserId</t>
   </si>
@@ -52,6 +53,24 @@
   </si>
   <si>
     <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>tele</t>
+  </si>
+  <si>
+    <t>marketing</t>
   </si>
 </sst>
 </file>
@@ -102,7 +121,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -113,6 +151,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{16A96413-6F49-4036-BD0E-AB021E8708F5}" name="Table2" displayName="Table2" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J2" xr:uid="{D3EC4FED-143B-495F-88C6-EDE6D2D2F8E9}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{A6C7AD10-BB00-4B27-9876-CFA559A1A2AB}" name="UserId"/>
+    <tableColumn id="2" xr3:uid="{AA810866-626D-40F0-9B4A-74E55D863A15}" name="Password"/>
+    <tableColumn id="3" xr3:uid="{97EDB55A-6F83-47C9-A2F7-1E7B9BB333A5}" name="UserName"/>
+    <tableColumn id="4" xr3:uid="{4C96017B-6357-47E2-8EC9-6F9EF09321B6}" name="AddressLine1"/>
+    <tableColumn id="5" xr3:uid="{2A408FC0-7991-4E68-8E9A-E2CCD835D7EA}" name="AddressLine2"/>
+    <tableColumn id="6" xr3:uid="{2B94A35F-A1B7-484D-8086-4A46429D3899}" name="PinOrZip"/>
+    <tableColumn id="7" xr3:uid="{FD4E4B0A-8C31-4757-AA66-FF99F79E2B2B}" name="LocalityOrVillage"/>
+    <tableColumn id="8" xr3:uid="{09D12868-0BB9-46E9-B929-86026C77D8CC}" name="SubDistrict"/>
+    <tableColumn id="9" xr3:uid="{74E93E0D-DA9D-4484-BCA6-5686C9DDFAA0}" name="MobileNumber"/>
+    <tableColumn id="10" xr3:uid="{20587061-5ABD-4C81-BC46-C7108A784C63}" name="Role"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3ECDAC5-A528-40EF-B62C-6B0D3D983F1C}" name="Table1" displayName="Table1" ref="A1:A6" totalsRowShown="0">
+  <autoFilter ref="A1:A6" xr:uid="{50A88674-2E8E-49DC-9C2F-1582159E847E}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B55BFC7D-11E6-4959-BF0F-23F07A3FD669}" name="Role"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,25 +479,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23DD7041-55E8-45E8-8B8E-231405707AAF}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="11.31640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="15.453125" customWidth="1"/>
     <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="7.953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" customWidth="1"/>
+    <col min="7" max="7" width="16.6796875" customWidth="1"/>
+    <col min="8" max="8" width="11.6796875" customWidth="1"/>
+    <col min="9" max="9" width="15.31640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +526,74 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{3BD73F26-10E4-4591-817A-DDD6EA11C66E}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D539C59-110D-4388-A93E-3CAA9C2186AB}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>